<commit_message>
re-did inputs directly from JS inputs. now there are more author_IDs than types
</commit_message>
<xml_diff>
--- a/2021.09.23 Author_Affiliations.xlsx
+++ b/2021.09.23 Author_Affiliations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josep\Documents\SNA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F8225A2-C475-451F-B541-1716B16C11E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0D79673-0281-4B53-8880-BC459B717DEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1536,22 +1536,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="7">
     <dxf>
-      <font>
-        <b val="0"/>
-      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
       <font>
@@ -1618,10 +1617,10 @@
   </sortState>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{B8F6899E-BF97-4624-ADC7-83920074EC56}" name="pmid" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{C0457102-F828-4C30-82CD-8BEF389FD604}" name="author_name" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{6CEA4693-F925-4FDD-B717-01E0762E6C6C}" name="author_id" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{C0457102-F828-4C30-82CD-8BEF389FD604}" name="author_name" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{6CEA4693-F925-4FDD-B717-01E0762E6C6C}" name="author_id" dataDxfId="0"/>
     <tableColumn id="4" xr3:uid="{0063641D-D9FA-4157-BDC7-912E55F7B109}" name="author_aff" dataDxfId="1"/>
-    <tableColumn id="5" xr3:uid="{7DE51D51-7617-45E4-9484-AF4F91788F61}" name="author_type" dataDxfId="0"/>
+    <tableColumn id="5" xr3:uid="{7DE51D51-7617-45E4-9484-AF4F91788F61}" name="author_type" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1951,7 +1950,7 @@
   <dimension ref="A1:F210"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="C210" sqref="C1:C210"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1970,7 +1969,7 @@
       <c r="B1" s="3" t="s">
         <v>482</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="4" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="3" t="s">
@@ -1987,7 +1986,7 @@
       <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D2" t="s">
@@ -2004,7 +2003,7 @@
       <c r="B3" t="s">
         <v>8</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D3" t="s">
@@ -2021,7 +2020,7 @@
       <c r="B4" t="s">
         <v>11</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="4" t="s">
         <v>12</v>
       </c>
       <c r="D4" t="s">
@@ -2038,7 +2037,7 @@
       <c r="B5" t="s">
         <v>14</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="4" t="s">
         <v>15</v>
       </c>
       <c r="D5" t="s">
@@ -2055,7 +2054,7 @@
       <c r="B6" t="s">
         <v>18</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="4" t="s">
         <v>19</v>
       </c>
       <c r="D6" t="s">
@@ -2072,7 +2071,7 @@
       <c r="B7" t="s">
         <v>20</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="4" t="s">
         <v>21</v>
       </c>
       <c r="D7" t="s">
@@ -2089,7 +2088,7 @@
       <c r="B8" t="s">
         <v>23</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="4" t="s">
         <v>24</v>
       </c>
       <c r="D8" t="s">
@@ -2106,7 +2105,7 @@
       <c r="B9" t="s">
         <v>26</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="4" t="s">
         <v>27</v>
       </c>
       <c r="D9" t="s">
@@ -2123,7 +2122,7 @@
       <c r="B10" t="s">
         <v>29</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="4" t="s">
         <v>30</v>
       </c>
       <c r="D10" t="s">
@@ -2140,7 +2139,7 @@
       <c r="B11" t="s">
         <v>32</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="4" t="s">
         <v>33</v>
       </c>
       <c r="D11" t="s">
@@ -2157,7 +2156,7 @@
       <c r="B12" t="s">
         <v>32</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="4" t="s">
         <v>33</v>
       </c>
       <c r="D12" t="s">
@@ -2174,7 +2173,7 @@
       <c r="B13" t="s">
         <v>35</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="4" t="s">
         <v>36</v>
       </c>
       <c r="D13" t="s">
@@ -2191,7 +2190,7 @@
       <c r="B14" t="s">
         <v>38</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="4" t="s">
         <v>39</v>
       </c>
       <c r="D14" t="s">
@@ -2208,7 +2207,7 @@
       <c r="B15" t="s">
         <v>41</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="4" t="s">
         <v>42</v>
       </c>
       <c r="D15" t="s">
@@ -2225,7 +2224,7 @@
       <c r="B16" t="s">
         <v>44</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="4" t="s">
         <v>45</v>
       </c>
       <c r="D16" t="s">
@@ -2242,7 +2241,7 @@
       <c r="B17" t="s">
         <v>47</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="4" t="s">
         <v>48</v>
       </c>
       <c r="D17" t="s">
@@ -2259,7 +2258,7 @@
       <c r="B18" t="s">
         <v>52</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="4" t="s">
         <v>50</v>
       </c>
       <c r="D18" t="s">
@@ -2276,7 +2275,7 @@
       <c r="B19" t="s">
         <v>52</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="4" t="s">
         <v>50</v>
       </c>
       <c r="D19" t="s">
@@ -2293,7 +2292,7 @@
       <c r="B20" t="s">
         <v>52</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="4" t="s">
         <v>50</v>
       </c>
       <c r="D20" t="s">
@@ -2310,7 +2309,7 @@
       <c r="B21" t="s">
         <v>52</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="4" t="s">
         <v>50</v>
       </c>
       <c r="D21" t="s">
@@ -2327,7 +2326,7 @@
       <c r="B22" t="s">
         <v>56</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" s="4" t="s">
         <v>57</v>
       </c>
       <c r="D22" t="s">
@@ -2344,7 +2343,7 @@
       <c r="B23" t="s">
         <v>61</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" s="4" t="s">
         <v>59</v>
       </c>
       <c r="D23" t="s">
@@ -2361,7 +2360,7 @@
       <c r="B24" t="s">
         <v>62</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C24" s="4" t="s">
         <v>63</v>
       </c>
       <c r="D24" t="s">
@@ -2378,7 +2377,7 @@
       <c r="B25" t="s">
         <v>67</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C25" s="4" t="s">
         <v>65</v>
       </c>
       <c r="D25" t="s">
@@ -2395,7 +2394,7 @@
       <c r="B26" t="s">
         <v>67</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C26" s="4" t="s">
         <v>65</v>
       </c>
       <c r="D26" t="s">
@@ -2412,7 +2411,7 @@
       <c r="B27" t="s">
         <v>67</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C27" s="4" t="s">
         <v>65</v>
       </c>
       <c r="D27" t="s">
@@ -2429,7 +2428,7 @@
       <c r="B28" t="s">
         <v>68</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C28" s="4" t="s">
         <v>69</v>
       </c>
       <c r="D28" t="s">
@@ -2446,7 +2445,7 @@
       <c r="B29" t="s">
         <v>68</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C29" s="4" t="s">
         <v>69</v>
       </c>
       <c r="D29" t="s">
@@ -2463,7 +2462,7 @@
       <c r="B30" t="s">
         <v>72</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C30" s="4" t="s">
         <v>73</v>
       </c>
       <c r="D30" t="s">
@@ -2480,7 +2479,7 @@
       <c r="B31" t="s">
         <v>74</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C31" s="4" t="s">
         <v>75</v>
       </c>
       <c r="D31" t="s">
@@ -2497,7 +2496,7 @@
       <c r="B32" t="s">
         <v>77</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C32" s="4" t="s">
         <v>78</v>
       </c>
       <c r="D32" t="s">
@@ -2514,7 +2513,7 @@
       <c r="B33" t="s">
         <v>80</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C33" s="4" t="s">
         <v>81</v>
       </c>
       <c r="D33" t="s">
@@ -2531,7 +2530,7 @@
       <c r="B34" t="s">
         <v>83</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C34" s="4" t="s">
         <v>84</v>
       </c>
       <c r="D34" t="s">
@@ -2548,7 +2547,7 @@
       <c r="B35" t="s">
         <v>86</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C35" s="4" t="s">
         <v>87</v>
       </c>
       <c r="D35" t="s">
@@ -2565,7 +2564,7 @@
       <c r="B36" t="s">
         <v>88</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C36" s="4" t="s">
         <v>89</v>
       </c>
       <c r="D36" t="s">
@@ -2582,7 +2581,7 @@
       <c r="B37" t="s">
         <v>90</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C37" s="4" t="s">
         <v>91</v>
       </c>
       <c r="D37" t="s">
@@ -2599,7 +2598,7 @@
       <c r="B38" t="s">
         <v>93</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C38" s="4" t="s">
         <v>94</v>
       </c>
       <c r="D38" t="s">
@@ -2616,7 +2615,7 @@
       <c r="B39" t="s">
         <v>95</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C39" s="4" t="s">
         <v>96</v>
       </c>
       <c r="D39" t="s">
@@ -2633,7 +2632,7 @@
       <c r="B40" t="s">
         <v>98</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C40" s="4" t="s">
         <v>99</v>
       </c>
       <c r="D40" t="s">
@@ -2650,7 +2649,7 @@
       <c r="B41" t="s">
         <v>102</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C41" s="4" t="s">
         <v>103</v>
       </c>
       <c r="D41" t="s">
@@ -2667,7 +2666,7 @@
       <c r="B42" t="s">
         <v>105</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C42" s="4" t="s">
         <v>106</v>
       </c>
       <c r="D42" t="s">
@@ -2684,7 +2683,7 @@
       <c r="B43" t="s">
         <v>107</v>
       </c>
-      <c r="C43" t="s">
+      <c r="C43" s="4" t="s">
         <v>108</v>
       </c>
       <c r="D43" t="s">
@@ -2701,7 +2700,7 @@
       <c r="B44" t="s">
         <v>110</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C44" s="4" t="s">
         <v>111</v>
       </c>
       <c r="D44" t="s">
@@ -2718,7 +2717,7 @@
       <c r="B45" t="s">
         <v>113</v>
       </c>
-      <c r="C45" t="s">
+      <c r="C45" s="4" t="s">
         <v>114</v>
       </c>
       <c r="D45" t="s">
@@ -2735,7 +2734,7 @@
       <c r="B46" t="s">
         <v>115</v>
       </c>
-      <c r="C46" t="s">
+      <c r="C46" s="4" t="s">
         <v>116</v>
       </c>
       <c r="D46" t="s">
@@ -2752,7 +2751,7 @@
       <c r="B47" t="s">
         <v>118</v>
       </c>
-      <c r="C47" t="s">
+      <c r="C47" s="4" t="s">
         <v>119</v>
       </c>
       <c r="D47" t="s">
@@ -2769,7 +2768,7 @@
       <c r="B48" t="s">
         <v>121</v>
       </c>
-      <c r="C48" t="s">
+      <c r="C48" s="4" t="s">
         <v>122</v>
       </c>
       <c r="D48" t="s">
@@ -2786,7 +2785,7 @@
       <c r="B49" t="s">
         <v>123</v>
       </c>
-      <c r="C49" t="s">
+      <c r="C49" s="4" t="s">
         <v>124</v>
       </c>
       <c r="D49" t="s">
@@ -2803,7 +2802,7 @@
       <c r="B50" t="s">
         <v>126</v>
       </c>
-      <c r="C50" t="s">
+      <c r="C50" s="4" t="s">
         <v>127</v>
       </c>
       <c r="D50" t="s">
@@ -2820,7 +2819,7 @@
       <c r="B51" t="s">
         <v>128</v>
       </c>
-      <c r="C51" t="s">
+      <c r="C51" s="4" t="s">
         <v>129</v>
       </c>
       <c r="D51" t="s">
@@ -2837,7 +2836,7 @@
       <c r="B52" t="s">
         <v>131</v>
       </c>
-      <c r="C52" t="s">
+      <c r="C52" s="4" t="s">
         <v>132</v>
       </c>
       <c r="D52" t="s">
@@ -2854,7 +2853,7 @@
       <c r="B53" t="s">
         <v>131</v>
       </c>
-      <c r="C53" t="s">
+      <c r="C53" s="4" t="s">
         <v>132</v>
       </c>
       <c r="D53" t="s">
@@ -2871,7 +2870,7 @@
       <c r="B54" t="s">
         <v>131</v>
       </c>
-      <c r="C54" t="s">
+      <c r="C54" s="4" t="s">
         <v>132</v>
       </c>
       <c r="D54" t="s">
@@ -2888,7 +2887,7 @@
       <c r="B55" t="s">
         <v>131</v>
       </c>
-      <c r="C55" t="s">
+      <c r="C55" s="4" t="s">
         <v>132</v>
       </c>
       <c r="D55" t="s">
@@ -2905,7 +2904,7 @@
       <c r="B56" t="s">
         <v>133</v>
       </c>
-      <c r="C56" t="s">
+      <c r="C56" s="4" t="s">
         <v>134</v>
       </c>
       <c r="D56" t="s">
@@ -2922,7 +2921,7 @@
       <c r="B57" t="s">
         <v>136</v>
       </c>
-      <c r="C57" t="s">
+      <c r="C57" s="4" t="s">
         <v>137</v>
       </c>
       <c r="D57" t="s">
@@ -2939,7 +2938,7 @@
       <c r="B58" t="s">
         <v>138</v>
       </c>
-      <c r="C58" t="s">
+      <c r="C58" s="4" t="s">
         <v>139</v>
       </c>
       <c r="D58" t="s">
@@ -2956,7 +2955,7 @@
       <c r="B59" t="s">
         <v>140</v>
       </c>
-      <c r="C59" t="s">
+      <c r="C59" s="4" t="s">
         <v>141</v>
       </c>
       <c r="D59" t="s">
@@ -2973,7 +2972,7 @@
       <c r="B60" t="s">
         <v>143</v>
       </c>
-      <c r="C60" t="s">
+      <c r="C60" s="4" t="s">
         <v>144</v>
       </c>
       <c r="D60" t="s">
@@ -2990,7 +2989,7 @@
       <c r="B61" t="s">
         <v>145</v>
       </c>
-      <c r="C61" t="s">
+      <c r="C61" s="4" t="s">
         <v>146</v>
       </c>
       <c r="D61" t="s">
@@ -3007,7 +3006,7 @@
       <c r="B62" t="s">
         <v>147</v>
       </c>
-      <c r="C62" t="s">
+      <c r="C62" s="4" t="s">
         <v>148</v>
       </c>
       <c r="D62" t="s">
@@ -3024,7 +3023,7 @@
       <c r="B63" t="s">
         <v>150</v>
       </c>
-      <c r="C63" t="s">
+      <c r="C63" s="4" t="s">
         <v>151</v>
       </c>
       <c r="D63" t="s">
@@ -3041,7 +3040,7 @@
       <c r="B64" t="s">
         <v>155</v>
       </c>
-      <c r="C64" t="s">
+      <c r="C64" s="4" t="s">
         <v>152</v>
       </c>
       <c r="D64" t="s">
@@ -3058,7 +3057,7 @@
       <c r="B65" t="s">
         <v>155</v>
       </c>
-      <c r="C65" t="s">
+      <c r="C65" s="4" t="s">
         <v>152</v>
       </c>
       <c r="D65" t="s">
@@ -3075,7 +3074,7 @@
       <c r="B66" t="s">
         <v>156</v>
       </c>
-      <c r="C66" t="s">
+      <c r="C66" s="4" t="s">
         <v>157</v>
       </c>
       <c r="D66" t="s">
@@ -3092,7 +3091,7 @@
       <c r="B67" t="s">
         <v>159</v>
       </c>
-      <c r="C67" t="s">
+      <c r="C67" s="4" t="s">
         <v>160</v>
       </c>
       <c r="D67" t="s">
@@ -3109,7 +3108,7 @@
       <c r="B68" t="s">
         <v>163</v>
       </c>
-      <c r="C68" t="s">
+      <c r="C68" s="4" t="s">
         <v>164</v>
       </c>
       <c r="D68" t="s">
@@ -3126,7 +3125,7 @@
       <c r="B69" t="s">
         <v>170</v>
       </c>
-      <c r="C69" t="s">
+      <c r="C69" s="4" t="s">
         <v>166</v>
       </c>
       <c r="D69" t="s">
@@ -3143,7 +3142,7 @@
       <c r="B70" t="s">
         <v>170</v>
       </c>
-      <c r="C70" t="s">
+      <c r="C70" s="4" t="s">
         <v>166</v>
       </c>
       <c r="D70" t="s">
@@ -3160,7 +3159,7 @@
       <c r="B71" t="s">
         <v>170</v>
       </c>
-      <c r="C71" t="s">
+      <c r="C71" s="4" t="s">
         <v>166</v>
       </c>
       <c r="D71" t="s">
@@ -3177,7 +3176,7 @@
       <c r="B72" t="s">
         <v>170</v>
       </c>
-      <c r="C72" t="s">
+      <c r="C72" s="4" t="s">
         <v>166</v>
       </c>
       <c r="D72" t="s">
@@ -3194,7 +3193,7 @@
       <c r="B73" t="s">
         <v>172</v>
       </c>
-      <c r="C73" t="s">
+      <c r="C73" s="4" t="s">
         <v>173</v>
       </c>
       <c r="D73" t="s">
@@ -3211,7 +3210,7 @@
       <c r="B74" t="s">
         <v>174</v>
       </c>
-      <c r="C74" t="s">
+      <c r="C74" s="4" t="s">
         <v>175</v>
       </c>
       <c r="D74" t="s">
@@ -3228,7 +3227,7 @@
       <c r="B75" t="s">
         <v>177</v>
       </c>
-      <c r="C75" t="s">
+      <c r="C75" s="4" t="s">
         <v>178</v>
       </c>
       <c r="D75" t="s">
@@ -3245,7 +3244,7 @@
       <c r="B76" t="s">
         <v>180</v>
       </c>
-      <c r="C76" t="s">
+      <c r="C76" s="4" t="s">
         <v>181</v>
       </c>
       <c r="D76" t="s">
@@ -3262,7 +3261,7 @@
       <c r="B77" t="s">
         <v>180</v>
       </c>
-      <c r="C77" t="s">
+      <c r="C77" s="4" t="s">
         <v>181</v>
       </c>
       <c r="D77" t="s">
@@ -3279,7 +3278,7 @@
       <c r="B78" t="s">
         <v>184</v>
       </c>
-      <c r="C78" t="s">
+      <c r="C78" s="4" t="s">
         <v>185</v>
       </c>
       <c r="D78" t="s">
@@ -3296,7 +3295,7 @@
       <c r="B79" t="s">
         <v>186</v>
       </c>
-      <c r="C79" t="s">
+      <c r="C79" s="4" t="s">
         <v>187</v>
       </c>
       <c r="D79" t="s">
@@ -3313,7 +3312,7 @@
       <c r="B80" t="s">
         <v>189</v>
       </c>
-      <c r="C80" t="s">
+      <c r="C80" s="4" t="s">
         <v>190</v>
       </c>
       <c r="D80" t="s">
@@ -3330,7 +3329,7 @@
       <c r="B81" t="s">
         <v>192</v>
       </c>
-      <c r="C81" t="s">
+      <c r="C81" s="4" t="s">
         <v>193</v>
       </c>
       <c r="D81" t="s">
@@ -3347,7 +3346,7 @@
       <c r="B82" t="s">
         <v>192</v>
       </c>
-      <c r="C82" t="s">
+      <c r="C82" s="4" t="s">
         <v>193</v>
       </c>
       <c r="D82" t="s">
@@ -3364,7 +3363,7 @@
       <c r="B83" t="s">
         <v>196</v>
       </c>
-      <c r="C83" t="s">
+      <c r="C83" s="4" t="s">
         <v>197</v>
       </c>
       <c r="D83" t="s">
@@ -3381,7 +3380,7 @@
       <c r="B84" t="s">
         <v>199</v>
       </c>
-      <c r="C84" t="s">
+      <c r="C84" s="4" t="s">
         <v>200</v>
       </c>
       <c r="D84" t="s">
@@ -3398,7 +3397,7 @@
       <c r="B85" t="s">
         <v>202</v>
       </c>
-      <c r="C85" t="s">
+      <c r="C85" s="4" t="s">
         <v>203</v>
       </c>
       <c r="D85" t="s">
@@ -3415,7 +3414,7 @@
       <c r="B86" t="s">
         <v>205</v>
       </c>
-      <c r="C86" t="s">
+      <c r="C86" s="4" t="s">
         <v>206</v>
       </c>
       <c r="D86" t="s">
@@ -3432,7 +3431,7 @@
       <c r="B87" t="s">
         <v>207</v>
       </c>
-      <c r="C87" t="s">
+      <c r="C87" s="4" t="s">
         <v>208</v>
       </c>
       <c r="D87" t="s">
@@ -3449,7 +3448,7 @@
       <c r="B88" t="s">
         <v>212</v>
       </c>
-      <c r="C88" t="s">
+      <c r="C88" s="4" t="s">
         <v>210</v>
       </c>
       <c r="D88" t="s">
@@ -3466,7 +3465,7 @@
       <c r="B89" t="s">
         <v>213</v>
       </c>
-      <c r="C89" t="s">
+      <c r="C89" s="4" t="s">
         <v>214</v>
       </c>
       <c r="D89" t="s">
@@ -3483,7 +3482,7 @@
       <c r="B90" t="s">
         <v>216</v>
       </c>
-      <c r="C90" t="s">
+      <c r="C90" s="4" t="s">
         <v>217</v>
       </c>
       <c r="D90" t="s">
@@ -3500,7 +3499,7 @@
       <c r="B91" t="s">
         <v>218</v>
       </c>
-      <c r="C91" t="s">
+      <c r="C91" s="4" t="s">
         <v>219</v>
       </c>
       <c r="D91" t="s">
@@ -3517,7 +3516,7 @@
       <c r="B92" t="s">
         <v>221</v>
       </c>
-      <c r="C92" t="s">
+      <c r="C92" s="4" t="s">
         <v>222</v>
       </c>
       <c r="D92" t="s">
@@ -3534,7 +3533,7 @@
       <c r="B93" t="s">
         <v>223</v>
       </c>
-      <c r="C93" t="s">
+      <c r="C93" s="4" t="s">
         <v>224</v>
       </c>
       <c r="D93" t="s">
@@ -3551,7 +3550,7 @@
       <c r="B94" t="s">
         <v>226</v>
       </c>
-      <c r="C94" t="s">
+      <c r="C94" s="4" t="s">
         <v>227</v>
       </c>
       <c r="D94" t="s">
@@ -3568,7 +3567,7 @@
       <c r="B95" t="s">
         <v>229</v>
       </c>
-      <c r="C95" t="s">
+      <c r="C95" s="4" t="s">
         <v>230</v>
       </c>
       <c r="D95" t="s">
@@ -3585,7 +3584,7 @@
       <c r="B96" t="s">
         <v>232</v>
       </c>
-      <c r="C96" t="s">
+      <c r="C96" s="4" t="s">
         <v>233</v>
       </c>
       <c r="D96" t="s">
@@ -3602,7 +3601,7 @@
       <c r="B97" t="s">
         <v>234</v>
       </c>
-      <c r="C97" t="s">
+      <c r="C97" s="4" t="s">
         <v>235</v>
       </c>
       <c r="D97" t="s">
@@ -3619,7 +3618,7 @@
       <c r="B98" t="s">
         <v>237</v>
       </c>
-      <c r="C98" t="s">
+      <c r="C98" s="4" t="s">
         <v>238</v>
       </c>
       <c r="D98" t="s">
@@ -3636,7 +3635,7 @@
       <c r="B99" t="s">
         <v>240</v>
       </c>
-      <c r="C99" t="s">
+      <c r="C99" s="4" t="s">
         <v>241</v>
       </c>
       <c r="D99" t="s">
@@ -3653,7 +3652,7 @@
       <c r="B100" t="s">
         <v>242</v>
       </c>
-      <c r="C100" t="s">
+      <c r="C100" s="4" t="s">
         <v>243</v>
       </c>
       <c r="D100" t="s">
@@ -3670,7 +3669,7 @@
       <c r="B101" t="s">
         <v>244</v>
       </c>
-      <c r="C101" t="s">
+      <c r="C101" s="4" t="s">
         <v>245</v>
       </c>
       <c r="D101" t="s">
@@ -3687,7 +3686,7 @@
       <c r="B102" t="s">
         <v>247</v>
       </c>
-      <c r="C102" t="s">
+      <c r="C102" s="4" t="s">
         <v>248</v>
       </c>
       <c r="D102" t="s">
@@ -3704,7 +3703,7 @@
       <c r="B103" t="s">
         <v>250</v>
       </c>
-      <c r="C103" t="s">
+      <c r="C103" s="4" t="s">
         <v>251</v>
       </c>
       <c r="D103" t="s">
@@ -3721,7 +3720,7 @@
       <c r="B104" t="s">
         <v>253</v>
       </c>
-      <c r="C104" t="s">
+      <c r="C104" s="4" t="s">
         <v>254</v>
       </c>
       <c r="D104" t="s">
@@ -3738,7 +3737,7 @@
       <c r="B105" t="s">
         <v>253</v>
       </c>
-      <c r="C105" t="s">
+      <c r="C105" s="4" t="s">
         <v>254</v>
       </c>
       <c r="D105" t="s">
@@ -3755,7 +3754,7 @@
       <c r="B106" t="s">
         <v>257</v>
       </c>
-      <c r="C106" t="s">
+      <c r="C106" s="4" t="s">
         <v>258</v>
       </c>
       <c r="D106" t="s">
@@ -3772,7 +3771,7 @@
       <c r="B107" t="s">
         <v>259</v>
       </c>
-      <c r="C107" t="s">
+      <c r="C107" s="4" t="s">
         <v>260</v>
       </c>
       <c r="D107" t="s">
@@ -3789,7 +3788,7 @@
       <c r="B108" t="s">
         <v>262</v>
       </c>
-      <c r="C108" t="s">
+      <c r="C108" s="4" t="s">
         <v>263</v>
       </c>
       <c r="D108" t="s">
@@ -3806,7 +3805,7 @@
       <c r="B109" t="s">
         <v>264</v>
       </c>
-      <c r="C109" t="s">
+      <c r="C109" s="4" t="s">
         <v>265</v>
       </c>
       <c r="D109" t="s">
@@ -3823,7 +3822,7 @@
       <c r="B110" t="s">
         <v>266</v>
       </c>
-      <c r="C110" t="s">
+      <c r="C110" s="4" t="s">
         <v>267</v>
       </c>
       <c r="D110" t="s">
@@ -3840,7 +3839,7 @@
       <c r="B111" t="s">
         <v>268</v>
       </c>
-      <c r="C111" t="s">
+      <c r="C111" s="4" t="s">
         <v>269</v>
       </c>
       <c r="D111" t="s">
@@ -3857,7 +3856,7 @@
       <c r="B112" t="s">
         <v>271</v>
       </c>
-      <c r="C112" t="s">
+      <c r="C112" s="4" t="s">
         <v>272</v>
       </c>
       <c r="D112" t="s">
@@ -3874,7 +3873,7 @@
       <c r="B113" t="s">
         <v>274</v>
       </c>
-      <c r="C113" t="s">
+      <c r="C113" s="4" t="s">
         <v>275</v>
       </c>
       <c r="D113" t="s">
@@ -3891,7 +3890,7 @@
       <c r="B114" t="s">
         <v>277</v>
       </c>
-      <c r="C114" t="s">
+      <c r="C114" s="4" t="s">
         <v>278</v>
       </c>
       <c r="D114" t="s">
@@ -3908,7 +3907,7 @@
       <c r="B115" s="1" t="s">
         <v>279</v>
       </c>
-      <c r="C115" s="1">
+      <c r="C115" s="4">
         <v>36731316800</v>
       </c>
       <c r="D115" s="1" t="s">
@@ -3925,7 +3924,7 @@
       <c r="B116" t="s">
         <v>281</v>
       </c>
-      <c r="C116" t="s">
+      <c r="C116" s="4" t="s">
         <v>282</v>
       </c>
       <c r="D116" t="s">
@@ -3942,7 +3941,7 @@
       <c r="B117" t="s">
         <v>283</v>
       </c>
-      <c r="C117" t="s">
+      <c r="C117" s="4" t="s">
         <v>284</v>
       </c>
       <c r="D117" t="s">
@@ -3959,7 +3958,7 @@
       <c r="B118" t="s">
         <v>288</v>
       </c>
-      <c r="C118" t="s">
+      <c r="C118" s="4" t="s">
         <v>286</v>
       </c>
       <c r="D118" t="s">
@@ -3976,7 +3975,7 @@
       <c r="B119" t="s">
         <v>288</v>
       </c>
-      <c r="C119" t="s">
+      <c r="C119" s="4" t="s">
         <v>286</v>
       </c>
       <c r="D119" t="s">
@@ -3993,7 +3992,7 @@
       <c r="B120" t="s">
         <v>290</v>
       </c>
-      <c r="C120" t="s">
+      <c r="C120" s="4" t="s">
         <v>291</v>
       </c>
       <c r="D120" t="s">
@@ -4010,7 +4009,7 @@
       <c r="B121" t="s">
         <v>292</v>
       </c>
-      <c r="C121" t="s">
+      <c r="C121" s="4" t="s">
         <v>293</v>
       </c>
       <c r="D121" t="s">
@@ -4027,7 +4026,7 @@
       <c r="B122" t="s">
         <v>294</v>
       </c>
-      <c r="C122" t="s">
+      <c r="C122" s="4" t="s">
         <v>295</v>
       </c>
       <c r="D122" t="s">
@@ -4044,7 +4043,7 @@
       <c r="B123" t="s">
         <v>296</v>
       </c>
-      <c r="C123" t="s">
+      <c r="C123" s="4" t="s">
         <v>297</v>
       </c>
       <c r="D123" t="s">
@@ -4061,7 +4060,7 @@
       <c r="B124" t="s">
         <v>298</v>
       </c>
-      <c r="C124" t="s">
+      <c r="C124" s="4" t="s">
         <v>299</v>
       </c>
       <c r="D124" t="s">
@@ -4078,7 +4077,7 @@
       <c r="B125" t="s">
         <v>302</v>
       </c>
-      <c r="C125" t="s">
+      <c r="C125" s="4" t="s">
         <v>301</v>
       </c>
       <c r="D125" t="s">
@@ -4095,7 +4094,7 @@
       <c r="B126" t="s">
         <v>302</v>
       </c>
-      <c r="C126" t="s">
+      <c r="C126" s="4" t="s">
         <v>301</v>
       </c>
       <c r="D126" t="s">
@@ -4112,7 +4111,7 @@
       <c r="B127" t="s">
         <v>303</v>
       </c>
-      <c r="C127" t="s">
+      <c r="C127" s="4" t="s">
         <v>304</v>
       </c>
       <c r="D127" t="s">
@@ -4129,7 +4128,7 @@
       <c r="B128" t="s">
         <v>306</v>
       </c>
-      <c r="C128" t="s">
+      <c r="C128" s="4" t="s">
         <v>307</v>
       </c>
       <c r="D128" t="s">
@@ -4146,7 +4145,7 @@
       <c r="B129" t="s">
         <v>308</v>
       </c>
-      <c r="C129" t="s">
+      <c r="C129" s="4" t="s">
         <v>309</v>
       </c>
       <c r="D129" t="s">
@@ -4163,7 +4162,7 @@
       <c r="B130" t="s">
         <v>308</v>
       </c>
-      <c r="C130" t="s">
+      <c r="C130" s="4" t="s">
         <v>309</v>
       </c>
       <c r="D130" t="s">
@@ -4180,7 +4179,7 @@
       <c r="B131" t="s">
         <v>308</v>
       </c>
-      <c r="C131" t="s">
+      <c r="C131" s="4" t="s">
         <v>309</v>
       </c>
       <c r="D131" t="s">
@@ -4197,7 +4196,7 @@
       <c r="B132" t="s">
         <v>308</v>
       </c>
-      <c r="C132" t="s">
+      <c r="C132" s="4" t="s">
         <v>309</v>
       </c>
       <c r="D132" t="s">
@@ -4214,7 +4213,7 @@
       <c r="B133" t="s">
         <v>310</v>
       </c>
-      <c r="C133" t="s">
+      <c r="C133" s="4" t="s">
         <v>311</v>
       </c>
       <c r="D133" t="s">
@@ -4231,7 +4230,7 @@
       <c r="B134" t="s">
         <v>313</v>
       </c>
-      <c r="C134" t="s">
+      <c r="C134" s="4" t="s">
         <v>312</v>
       </c>
       <c r="D134" t="s">
@@ -4248,7 +4247,7 @@
       <c r="B135" t="s">
         <v>315</v>
       </c>
-      <c r="C135" t="s">
+      <c r="C135" s="4" t="s">
         <v>316</v>
       </c>
       <c r="D135" t="s">
@@ -4265,7 +4264,7 @@
       <c r="B136" t="s">
         <v>318</v>
       </c>
-      <c r="C136" t="s">
+      <c r="C136" s="4" t="s">
         <v>319</v>
       </c>
       <c r="D136" t="s">
@@ -4282,7 +4281,7 @@
       <c r="B137" t="s">
         <v>321</v>
       </c>
-      <c r="C137" t="s">
+      <c r="C137" s="4" t="s">
         <v>322</v>
       </c>
       <c r="D137" t="s">
@@ -4299,7 +4298,7 @@
       <c r="B138" t="s">
         <v>324</v>
       </c>
-      <c r="C138" t="s">
+      <c r="C138" s="4" t="s">
         <v>325</v>
       </c>
       <c r="D138" t="s">
@@ -4316,7 +4315,7 @@
       <c r="B139" t="s">
         <v>327</v>
       </c>
-      <c r="C139" t="s">
+      <c r="C139" s="4" t="s">
         <v>328</v>
       </c>
       <c r="D139" t="s">
@@ -4333,7 +4332,7 @@
       <c r="B140" t="s">
         <v>330</v>
       </c>
-      <c r="C140" t="s">
+      <c r="C140" s="4" t="s">
         <v>331</v>
       </c>
       <c r="D140" t="s">
@@ -4350,7 +4349,7 @@
       <c r="B141" t="s">
         <v>330</v>
       </c>
-      <c r="C141" t="s">
+      <c r="C141" s="4" t="s">
         <v>331</v>
       </c>
       <c r="D141" t="s">
@@ -4367,7 +4366,7 @@
       <c r="B142" t="s">
         <v>333</v>
       </c>
-      <c r="C142" t="s">
+      <c r="C142" s="4" t="s">
         <v>334</v>
       </c>
       <c r="D142" t="s">
@@ -4384,7 +4383,7 @@
       <c r="B143" t="s">
         <v>336</v>
       </c>
-      <c r="C143" t="s">
+      <c r="C143" s="4" t="s">
         <v>337</v>
       </c>
       <c r="D143" t="s">
@@ -4401,7 +4400,7 @@
       <c r="B144" t="s">
         <v>338</v>
       </c>
-      <c r="C144" t="s">
+      <c r="C144" s="4" t="s">
         <v>339</v>
       </c>
       <c r="D144" t="s">
@@ -4418,7 +4417,7 @@
       <c r="B145" t="s">
         <v>341</v>
       </c>
-      <c r="C145" t="s">
+      <c r="C145" s="4" t="s">
         <v>342</v>
       </c>
       <c r="D145" t="s">
@@ -4435,7 +4434,7 @@
       <c r="B146" t="s">
         <v>344</v>
       </c>
-      <c r="C146" t="s">
+      <c r="C146" s="4" t="s">
         <v>345</v>
       </c>
       <c r="D146" t="s">
@@ -4452,7 +4451,7 @@
       <c r="B147" t="s">
         <v>347</v>
       </c>
-      <c r="C147" t="s">
+      <c r="C147" s="4" t="s">
         <v>348</v>
       </c>
       <c r="D147" t="s">
@@ -4469,7 +4468,7 @@
       <c r="B148" t="s">
         <v>349</v>
       </c>
-      <c r="C148" t="s">
+      <c r="C148" s="4" t="s">
         <v>350</v>
       </c>
       <c r="D148" t="s">
@@ -4486,7 +4485,7 @@
       <c r="B149" t="s">
         <v>351</v>
       </c>
-      <c r="C149" t="s">
+      <c r="C149" s="4" t="s">
         <v>352</v>
       </c>
       <c r="D149" t="s">
@@ -4503,7 +4502,7 @@
       <c r="B150" t="s">
         <v>354</v>
       </c>
-      <c r="C150" t="s">
+      <c r="C150" s="4" t="s">
         <v>355</v>
       </c>
       <c r="D150" t="s">
@@ -4520,7 +4519,7 @@
       <c r="B151" t="s">
         <v>356</v>
       </c>
-      <c r="C151" t="s">
+      <c r="C151" s="4" t="s">
         <v>357</v>
       </c>
       <c r="D151" t="s">
@@ -4537,7 +4536,7 @@
       <c r="B152" t="s">
         <v>358</v>
       </c>
-      <c r="C152" t="s">
+      <c r="C152" s="4" t="s">
         <v>359</v>
       </c>
       <c r="D152" t="s">
@@ -4554,7 +4553,7 @@
       <c r="B153" t="s">
         <v>358</v>
       </c>
-      <c r="C153" t="s">
+      <c r="C153" s="4" t="s">
         <v>359</v>
       </c>
       <c r="D153" t="s">
@@ -4571,7 +4570,7 @@
       <c r="B154" t="s">
         <v>361</v>
       </c>
-      <c r="C154" t="s">
+      <c r="C154" s="4" t="s">
         <v>362</v>
       </c>
       <c r="D154" t="s">
@@ -4588,7 +4587,7 @@
       <c r="B155" t="s">
         <v>363</v>
       </c>
-      <c r="C155" t="s">
+      <c r="C155" s="4" t="s">
         <v>364</v>
       </c>
       <c r="D155" t="s">
@@ -4605,7 +4604,7 @@
       <c r="B156" t="s">
         <v>366</v>
       </c>
-      <c r="C156" t="s">
+      <c r="C156" s="4" t="s">
         <v>367</v>
       </c>
       <c r="D156" t="s">
@@ -4622,7 +4621,7 @@
       <c r="B157" t="s">
         <v>368</v>
       </c>
-      <c r="C157" t="s">
+      <c r="C157" s="4" t="s">
         <v>369</v>
       </c>
       <c r="D157" t="s">
@@ -4639,7 +4638,7 @@
       <c r="B158" t="s">
         <v>370</v>
       </c>
-      <c r="C158" t="s">
+      <c r="C158" s="4" t="s">
         <v>371</v>
       </c>
       <c r="D158" t="s">
@@ -4656,7 +4655,7 @@
       <c r="B159" t="s">
         <v>373</v>
       </c>
-      <c r="C159" t="s">
+      <c r="C159" s="4" t="s">
         <v>374</v>
       </c>
       <c r="D159" t="s">
@@ -4673,7 +4672,7 @@
       <c r="B160" t="s">
         <v>376</v>
       </c>
-      <c r="C160" t="s">
+      <c r="C160" s="4" t="s">
         <v>377</v>
       </c>
       <c r="D160" t="s">
@@ -4690,7 +4689,7 @@
       <c r="B161" t="s">
         <v>379</v>
       </c>
-      <c r="C161" t="s">
+      <c r="C161" s="4" t="s">
         <v>380</v>
       </c>
       <c r="D161" t="s">
@@ -4707,7 +4706,7 @@
       <c r="B162" t="s">
         <v>381</v>
       </c>
-      <c r="C162" t="s">
+      <c r="C162" s="4" t="s">
         <v>382</v>
       </c>
       <c r="D162" t="s">
@@ -4724,7 +4723,7 @@
       <c r="B163" t="s">
         <v>384</v>
       </c>
-      <c r="C163" t="s">
+      <c r="C163" s="4" t="s">
         <v>385</v>
       </c>
       <c r="D163" t="s">
@@ -4741,7 +4740,7 @@
       <c r="B164" t="s">
         <v>386</v>
       </c>
-      <c r="C164" t="s">
+      <c r="C164" s="4" t="s">
         <v>387</v>
       </c>
       <c r="D164" t="s">
@@ -4758,7 +4757,7 @@
       <c r="B165" t="s">
         <v>389</v>
       </c>
-      <c r="C165" t="s">
+      <c r="C165" s="4" t="s">
         <v>390</v>
       </c>
       <c r="D165" t="s">
@@ -4775,7 +4774,7 @@
       <c r="B166" t="s">
         <v>391</v>
       </c>
-      <c r="C166" t="s">
+      <c r="C166" s="4" t="s">
         <v>392</v>
       </c>
       <c r="D166" t="s">
@@ -4792,7 +4791,7 @@
       <c r="B167" t="s">
         <v>394</v>
       </c>
-      <c r="C167" t="s">
+      <c r="C167" s="4" t="s">
         <v>395</v>
       </c>
       <c r="D167" t="s">
@@ -4809,7 +4808,7 @@
       <c r="B168" t="s">
         <v>396</v>
       </c>
-      <c r="C168" t="s">
+      <c r="C168" s="4" t="s">
         <v>397</v>
       </c>
       <c r="D168" t="s">
@@ -4826,7 +4825,7 @@
       <c r="B169" t="s">
         <v>399</v>
       </c>
-      <c r="C169" t="s">
+      <c r="C169" s="4" t="s">
         <v>400</v>
       </c>
       <c r="D169" t="s">
@@ -4843,7 +4842,7 @@
       <c r="B170" t="s">
         <v>402</v>
       </c>
-      <c r="C170" t="s">
+      <c r="C170" s="4" t="s">
         <v>403</v>
       </c>
       <c r="D170" t="s">
@@ -4860,7 +4859,7 @@
       <c r="B171" t="s">
         <v>404</v>
       </c>
-      <c r="C171" t="s">
+      <c r="C171" s="4" t="s">
         <v>405</v>
       </c>
       <c r="D171" t="s">
@@ -4877,7 +4876,7 @@
       <c r="B172" t="s">
         <v>406</v>
       </c>
-      <c r="C172" t="s">
+      <c r="C172" s="4" t="s">
         <v>407</v>
       </c>
       <c r="D172" t="s">
@@ -4894,7 +4893,7 @@
       <c r="B173" t="s">
         <v>408</v>
       </c>
-      <c r="C173" t="s">
+      <c r="C173" s="4" t="s">
         <v>409</v>
       </c>
       <c r="D173" t="s">
@@ -4911,7 +4910,7 @@
       <c r="B174" t="s">
         <v>410</v>
       </c>
-      <c r="C174" t="s">
+      <c r="C174" s="4" t="s">
         <v>411</v>
       </c>
       <c r="D174" t="s">
@@ -4928,7 +4927,7 @@
       <c r="B175" t="s">
         <v>412</v>
       </c>
-      <c r="C175" t="s">
+      <c r="C175" s="4" t="s">
         <v>413</v>
       </c>
       <c r="D175" t="s">
@@ -4945,7 +4944,7 @@
       <c r="B176" t="s">
         <v>414</v>
       </c>
-      <c r="C176" t="s">
+      <c r="C176" s="4" t="s">
         <v>415</v>
       </c>
       <c r="D176" t="s">
@@ -4962,7 +4961,7 @@
       <c r="B177" t="s">
         <v>417</v>
       </c>
-      <c r="C177" t="s">
+      <c r="C177" s="4" t="s">
         <v>418</v>
       </c>
       <c r="D177" t="s">
@@ -4979,7 +4978,7 @@
       <c r="B178" t="s">
         <v>419</v>
       </c>
-      <c r="C178" t="s">
+      <c r="C178" s="4" t="s">
         <v>420</v>
       </c>
       <c r="D178" t="s">
@@ -4996,7 +4995,7 @@
       <c r="B179" t="s">
         <v>422</v>
       </c>
-      <c r="C179" t="s">
+      <c r="C179" s="4" t="s">
         <v>423</v>
       </c>
       <c r="D179" t="s">
@@ -5013,7 +5012,7 @@
       <c r="B180" t="s">
         <v>424</v>
       </c>
-      <c r="C180" t="s">
+      <c r="C180" s="4" t="s">
         <v>425</v>
       </c>
       <c r="D180" t="s">
@@ -5030,7 +5029,7 @@
       <c r="B181" t="s">
         <v>426</v>
       </c>
-      <c r="C181" t="s">
+      <c r="C181" s="4" t="s">
         <v>427</v>
       </c>
       <c r="D181" t="s">
@@ -5047,7 +5046,7 @@
       <c r="B182" t="s">
         <v>429</v>
       </c>
-      <c r="C182" t="s">
+      <c r="C182" s="4" t="s">
         <v>430</v>
       </c>
       <c r="D182" t="s">
@@ -5064,7 +5063,7 @@
       <c r="B183" t="s">
         <v>431</v>
       </c>
-      <c r="C183" t="s">
+      <c r="C183" s="4" t="s">
         <v>432</v>
       </c>
       <c r="D183" t="s">
@@ -5081,7 +5080,7 @@
       <c r="B184" t="s">
         <v>434</v>
       </c>
-      <c r="C184" t="s">
+      <c r="C184" s="4" t="s">
         <v>435</v>
       </c>
       <c r="D184" t="s">
@@ -5098,7 +5097,7 @@
       <c r="B185" t="s">
         <v>436</v>
       </c>
-      <c r="C185" t="s">
+      <c r="C185" s="4" t="s">
         <v>437</v>
       </c>
       <c r="D185" t="s">
@@ -5115,7 +5114,7 @@
       <c r="B186" t="s">
         <v>438</v>
       </c>
-      <c r="C186" t="s">
+      <c r="C186" s="4" t="s">
         <v>439</v>
       </c>
       <c r="D186" t="s">
@@ -5132,7 +5131,7 @@
       <c r="B187" t="s">
         <v>438</v>
       </c>
-      <c r="C187" t="s">
+      <c r="C187" s="4" t="s">
         <v>439</v>
       </c>
       <c r="D187" t="s">
@@ -5149,7 +5148,7 @@
       <c r="B188" t="s">
         <v>440</v>
       </c>
-      <c r="C188" t="s">
+      <c r="C188" s="4" t="s">
         <v>441</v>
       </c>
       <c r="D188" t="s">
@@ -5166,7 +5165,7 @@
       <c r="B189" t="s">
         <v>442</v>
       </c>
-      <c r="C189" t="s">
+      <c r="C189" s="4" t="s">
         <v>443</v>
       </c>
       <c r="D189" t="s">
@@ -5183,7 +5182,7 @@
       <c r="B190" t="s">
         <v>445</v>
       </c>
-      <c r="C190" t="s">
+      <c r="C190" s="4" t="s">
         <v>446</v>
       </c>
       <c r="D190" t="s">
@@ -5200,7 +5199,7 @@
       <c r="B191" t="s">
         <v>447</v>
       </c>
-      <c r="C191" t="s">
+      <c r="C191" s="4" t="s">
         <v>448</v>
       </c>
       <c r="D191" t="s">
@@ -5217,7 +5216,7 @@
       <c r="B192" t="s">
         <v>450</v>
       </c>
-      <c r="C192" t="s">
+      <c r="C192" s="4" t="s">
         <v>451</v>
       </c>
       <c r="D192" t="s">
@@ -5234,7 +5233,7 @@
       <c r="B193" t="s">
         <v>452</v>
       </c>
-      <c r="C193" t="s">
+      <c r="C193" s="4" t="s">
         <v>453</v>
       </c>
       <c r="D193" t="s">
@@ -5251,7 +5250,7 @@
       <c r="B194" t="s">
         <v>454</v>
       </c>
-      <c r="C194" t="s">
+      <c r="C194" s="4" t="s">
         <v>455</v>
       </c>
       <c r="D194" t="s">
@@ -5268,7 +5267,7 @@
       <c r="B195" s="2" t="s">
         <v>457</v>
       </c>
-      <c r="C195" s="2">
+      <c r="C195" s="4">
         <v>57247761200</v>
       </c>
       <c r="D195" s="2" t="s">
@@ -5286,7 +5285,7 @@
       <c r="B196" t="s">
         <v>458</v>
       </c>
-      <c r="C196" t="s">
+      <c r="C196" s="4" t="s">
         <v>459</v>
       </c>
       <c r="D196" t="s">
@@ -5303,7 +5302,7 @@
       <c r="B197" t="s">
         <v>460</v>
       </c>
-      <c r="C197" t="s">
+      <c r="C197" s="4" t="s">
         <v>461</v>
       </c>
       <c r="D197" t="s">
@@ -5320,7 +5319,7 @@
       <c r="B198" t="s">
         <v>463</v>
       </c>
-      <c r="C198" t="s">
+      <c r="C198" s="4" t="s">
         <v>464</v>
       </c>
       <c r="D198" t="s">
@@ -5337,7 +5336,7 @@
       <c r="B199" t="s">
         <v>463</v>
       </c>
-      <c r="C199" t="s">
+      <c r="C199" s="4" t="s">
         <v>464</v>
       </c>
       <c r="D199" t="s">
@@ -5354,7 +5353,7 @@
       <c r="B200" t="s">
         <v>463</v>
       </c>
-      <c r="C200" t="s">
+      <c r="C200" s="4" t="s">
         <v>464</v>
       </c>
       <c r="D200" t="s">
@@ -5371,7 +5370,7 @@
       <c r="B201" t="s">
         <v>463</v>
       </c>
-      <c r="C201" t="s">
+      <c r="C201" s="4" t="s">
         <v>464</v>
       </c>
       <c r="D201" t="s">
@@ -5388,7 +5387,7 @@
       <c r="B202" t="s">
         <v>463</v>
       </c>
-      <c r="C202" t="s">
+      <c r="C202" s="4" t="s">
         <v>464</v>
       </c>
       <c r="D202" t="s">
@@ -5405,7 +5404,7 @@
       <c r="B203" t="s">
         <v>466</v>
       </c>
-      <c r="C203" t="s">
+      <c r="C203" s="4" t="s">
         <v>467</v>
       </c>
       <c r="D203" t="s">
@@ -5422,7 +5421,7 @@
       <c r="B204" t="s">
         <v>468</v>
       </c>
-      <c r="C204" t="s">
+      <c r="C204" s="4" t="s">
         <v>469</v>
       </c>
       <c r="D204" t="s">
@@ -5439,7 +5438,7 @@
       <c r="B205" t="s">
         <v>470</v>
       </c>
-      <c r="C205" t="s">
+      <c r="C205" s="4" t="s">
         <v>471</v>
       </c>
       <c r="D205" t="s">
@@ -5456,7 +5455,7 @@
       <c r="B206" t="s">
         <v>472</v>
       </c>
-      <c r="C206" t="s">
+      <c r="C206" s="4" t="s">
         <v>473</v>
       </c>
       <c r="D206" t="s">
@@ -5473,7 +5472,7 @@
       <c r="B207" t="s">
         <v>475</v>
       </c>
-      <c r="C207" t="s">
+      <c r="C207" s="4" t="s">
         <v>476</v>
       </c>
       <c r="D207" t="s">
@@ -5490,7 +5489,7 @@
       <c r="B208" t="s">
         <v>475</v>
       </c>
-      <c r="C208" t="s">
+      <c r="C208" s="4" t="s">
         <v>476</v>
       </c>
       <c r="D208" t="s">
@@ -5507,7 +5506,7 @@
       <c r="B209" t="s">
         <v>477</v>
       </c>
-      <c r="C209" t="s">
+      <c r="C209" s="4" t="s">
         <v>478</v>
       </c>
       <c r="D209" t="s">
@@ -5524,7 +5523,7 @@
       <c r="B210" t="s">
         <v>480</v>
       </c>
-      <c r="C210" t="s">
+      <c r="C210" s="4" t="s">
         <v>481</v>
       </c>
       <c r="D210" t="s">
@@ -5544,17 +5543,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="e5c03532-ca69-4eca-baa0-f6c5bcd6c094" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="57a8e7ef-4f20-414a-a2d4-5a9bd8d86111">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100CF80A72F950AB44BBD3F7B6758C7B51D" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b571fce440275f0622ff001093cb92ee">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="57a8e7ef-4f20-414a-a2d4-5a9bd8d86111" xmlns:ns3="e5c03532-ca69-4eca-baa0-f6c5bcd6c094" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f94315dc4d15cb105dea15baff015bd0" ns2:_="" ns3:_="">
     <xsd:import namespace="57a8e7ef-4f20-414a-a2d4-5a9bd8d86111"/>
@@ -5773,6 +5761,17 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="e5c03532-ca69-4eca-baa0-f6c5bcd6c094" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="57a8e7ef-4f20-414a-a2d4-5a9bd8d86111">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -5783,17 +5782,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2D06896F-B9E0-4410-A772-3EB1E1F27771}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="e5c03532-ca69-4eca-baa0-f6c5bcd6c094"/>
-    <ds:schemaRef ds:uri="57a8e7ef-4f20-414a-a2d4-5a9bd8d86111"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CC6D2546-0A27-4146-AB1D-352EBB352AFD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5812,6 +5800,17 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2D06896F-B9E0-4410-A772-3EB1E1F27771}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="e5c03532-ca69-4eca-baa0-f6c5bcd6c094"/>
+    <ds:schemaRef ds:uri="57a8e7ef-4f20-414a-a2d4-5a9bd8d86111"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ECF2A7D3-433A-4455-B95D-DBA96B4DDA19}">
   <ds:schemaRefs>

</xml_diff>